<commit_message>
Correct knit lab pdf
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordaninskeep/Documents/6_School/0_rs4500Lab/Lab 1/rs4500_Lab1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA191D8-61B3-B44D-B9C0-45140E89EBBB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEEE2B4F-582C-A445-A7F4-4559518FB051}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16180" yWindow="460" windowWidth="17420" windowHeight="16000" xr2:uid="{A7DE2093-C2D9-D545-AE28-3C6523133B80}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="26">
   <si>
     <t>type</t>
   </si>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF389C1C-8260-3245-93BC-A72D9B11A6D3}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -888,6 +888,9 @@
       <c r="C12" t="s">
         <v>11</v>
       </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
       <c r="G12" t="s">
         <v>3</v>
       </c>

</xml_diff>